<commit_message>
Create a hardware tester script in micropython
</commit_message>
<xml_diff>
--- a/hardware/electronics/Pico_Synth_Ali_BOM.xlsx
+++ b/hardware/electronics/Pico_Synth_Ali_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlame\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlame\Documents\MEEC\Hackerschool\PicoSynth\pico-synth\hardware\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9955BE84-F918-4552-9960-E832149A1C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7213CB20-5514-41CB-8A0C-793210701744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D2EBFBF8-8DB4-4F18-9325-C88CF28441A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>Ref</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Header Female (2.54 pitch)</t>
+  </si>
+  <si>
+    <t>Encomendado</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +273,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -349,26 +358,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -378,6 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -716,7 +724,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,17 +737,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8">
+      <c r="B1" s="6">
         <v>5</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="G1" t="s">
         <v>32</v>
       </c>
@@ -752,9 +760,7 @@
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="4"/>
       <c r="G2" t="s">
         <v>33</v>
       </c>
@@ -765,26 +771,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -812,7 +820,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -832,12 +840,12 @@
         <f>D9*E9</f>
         <v>10.95</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -855,12 +863,12 @@
         <f t="shared" ref="F10:F12" si="1">D10*E10</f>
         <v>10.95</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
@@ -878,7 +886,7 @@
         <f t="shared" si="1"/>
         <v>4.6000000000000005</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -901,12 +909,12 @@
         <f t="shared" si="1"/>
         <v>7.95</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -934,10 +942,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="1">
@@ -954,12 +962,12 @@
         <f>E16*D16/5</f>
         <v>5.91</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -979,12 +987,12 @@
         <f>E17</f>
         <v>2.11</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1004,12 +1012,12 @@
         <f>E18*D18/5</f>
         <v>9.8800000000000008</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1026,15 +1034,15 @@
         <v>1.44</v>
       </c>
       <c r="F19" s="1">
-        <f>E19</f>
+        <f t="shared" ref="F19:F24" si="2">E19</f>
         <v>1.44</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1044,22 +1052,22 @@
         <v>16</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" ref="D19:D27" si="2">C20*$B$1</f>
+        <f t="shared" ref="D20:D27" si="3">C20*$B$1</f>
         <v>80</v>
       </c>
       <c r="E20" s="1">
         <v>1.81</v>
       </c>
       <c r="F20" s="1">
-        <f>E20</f>
+        <f t="shared" si="2"/>
         <v>1.81</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1069,22 +1077,22 @@
         <v>16</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="E21" s="1">
         <v>1.39</v>
       </c>
       <c r="F21" s="1">
-        <f>E21</f>
+        <f t="shared" si="2"/>
         <v>1.39</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1094,14 +1102,14 @@
         <v>4</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="E22" s="1">
         <v>1.47</v>
       </c>
       <c r="F22" s="1">
-        <f>E22</f>
+        <f t="shared" si="2"/>
         <v>1.47</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1109,7 +1117,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1119,14 +1127,14 @@
         <v>1</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="E23" s="1">
         <v>1.46</v>
       </c>
       <c r="F23" s="1">
-        <f>E23</f>
+        <f t="shared" si="2"/>
         <v>1.46</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -1134,7 +1142,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1144,14 +1152,14 @@
         <v>4</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="E24" s="1">
         <v>1.24</v>
       </c>
       <c r="F24" s="1">
-        <f>E24</f>
+        <f t="shared" si="2"/>
         <v>1.24</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -1159,7 +1167,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1169,7 +1177,7 @@
         <v>28</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="E25" s="1">
@@ -1184,7 +1192,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1194,7 +1202,7 @@
         <v>12</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="E26" s="1">
@@ -1217,7 +1225,7 @@
         <v>69</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>345</v>
       </c>
       <c r="E27" s="3">
@@ -1227,17 +1235,17 @@
         <f>E27</f>
         <v>1.79</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1255,12 +1263,12 @@
         <f>E30</f>
         <v>5.54</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1268,7 +1276,7 @@
         <v>16</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" ref="D31:D32" si="3">C31*$B$1</f>
+        <f t="shared" ref="D31:D32" si="4">C31*$B$1</f>
         <v>80</v>
       </c>
       <c r="E31" s="1">
@@ -1278,7 +1286,7 @@
         <f>E31</f>
         <v>12.99</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1291,7 +1299,7 @@
         <v>16</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="E32" s="1">
@@ -1301,7 +1309,7 @@
         <f>E32*D32/20</f>
         <v>16.16</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>